<commit_message>
add Optimize Solvers implemetation
</commit_message>
<xml_diff>
--- a/SPP.xlsx
+++ b/SPP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
         <v>8680</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2658849990111776</v>
+        <v>0.2652231190004386</v>
       </c>
       <c r="E2" t="n">
         <v>20</v>
@@ -502,7 +502,7 @@
         <v>9853</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3087723379721865</v>
+        <v>0.3125638689962216</v>
       </c>
       <c r="E3" t="n">
         <v>20</v>
@@ -526,7 +526,7 @@
         <v>8792</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2049497480038553</v>
+        <v>0.2129374389769509</v>
       </c>
       <c r="E4" t="n">
         <v>20</v>
@@ -549,15 +549,939 @@
       <c r="C5" t="n">
         <v>30245</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
+      <c r="D5" t="n">
+        <v>3.673541600001045</v>
       </c>
       <c r="E5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HT05(c2p2)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2418</v>
+      </c>
+      <c r="C6" t="n">
+        <v>30680</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.888466086005792</v>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HT06(c2p3)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2416</v>
+      </c>
+      <c r="C7" t="n">
+        <v>30594</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8519042059779167</v>
+      </c>
+      <c r="E7" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>HT07(c3p1)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3677</v>
+      </c>
+      <c r="C8" t="n">
+        <v>60998</v>
+      </c>
+      <c r="D8" t="n">
+        <v>14.9961232499918</v>
+      </c>
+      <c r="E8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HT08(c3p2)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3890</v>
+      </c>
+      <c r="C9" t="n">
+        <v>66024</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>31</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>HT09(c3p3)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3681</v>
+      </c>
+      <c r="C10" t="n">
+        <v>61084</v>
+      </c>
+      <c r="D10" t="n">
+        <v>51.47719361400232</v>
+      </c>
+      <c r="E10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CGCUT01</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>900</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6810</v>
+      </c>
+      <c r="D11" t="n">
+        <v>515.0848403020063</v>
+      </c>
+      <c r="E11" t="n">
+        <v>17</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CGCUT02</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3926</v>
+      </c>
+      <c r="C12" t="n">
+        <v>67275</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>116</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CGCUT03</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>90225</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5126873</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1571</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GCUT01</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>7484</v>
+      </c>
+      <c r="C14" t="n">
+        <v>73085</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6.061176014016382</v>
+      </c>
+      <c r="E14" t="n">
+        <v>731</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GCUT02</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>26943</v>
+      </c>
+      <c r="C15" t="n">
+        <v>523850</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>1330</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>GCUT03</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>53654</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1557855</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1793</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>GCUT04</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>162970</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7904725</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>3369</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>NGCUT01</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>409</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2335</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.07082334998995066</v>
+      </c>
+      <c r="E18" t="n">
+        <v>20</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>NGCUT02</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1094</v>
+      </c>
+      <c r="C19" t="n">
+        <v>9398</v>
+      </c>
+      <c r="D19" t="n">
+        <v>9.377688505977858</v>
+      </c>
+      <c r="E19" t="n">
+        <v>29</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>NGCUT03</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1548</v>
+      </c>
+      <c r="C20" t="n">
+        <v>14952</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>30</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>NGCUT04</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>201</v>
+      </c>
+      <c r="C21" t="n">
+        <v>834</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.007145330018829554</v>
+      </c>
+      <c r="E21" t="n">
+        <v>12</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>NGCUT05</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>863</v>
+      </c>
+      <c r="C22" t="n">
+        <v>7011</v>
+      </c>
+      <c r="D22" t="n">
+        <v>192.9788152209949</v>
+      </c>
+      <c r="E22" t="n">
+        <v>30</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>NGCUT06</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>851</v>
+      </c>
+      <c r="C23" t="n">
+        <v>6554</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.2694387389929034</v>
+      </c>
+      <c r="E23" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>NGCUT07</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>316</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1628</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.02448407997144386</v>
+      </c>
+      <c r="E24" t="n">
+        <v>14</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>NGCUT08</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>858</v>
+      </c>
+      <c r="C25" t="n">
+        <v>7158</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.638874642958399</v>
+      </c>
+      <c r="E25" t="n">
+        <v>36</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>NGCUT09</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1689</v>
+      </c>
+      <c r="C26" t="n">
+        <v>19441</v>
+      </c>
+      <c r="D26" t="n">
+        <v>21.55591251503211</v>
+      </c>
+      <c r="E26" t="n">
+        <v>52</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>NGCUT10</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1106</v>
+      </c>
+      <c r="C27" t="n">
+        <v>10394</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4.948505807959009</v>
+      </c>
+      <c r="E27" t="n">
+        <v>62</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>NGCUT11</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1453</v>
+      </c>
+      <c r="C28" t="n">
+        <v>15600</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.05446800601203</v>
+      </c>
+      <c r="E28" t="n">
+        <v>59</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>NGCUT12</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2827</v>
+      </c>
+      <c r="C29" t="n">
+        <v>42019</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>80</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BENG01</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1685</v>
+      </c>
+      <c r="C30" t="n">
+        <v>18552</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.6063239469658583</v>
+      </c>
+      <c r="E30" t="n">
+        <v>30</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>BENG02</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6072</v>
+      </c>
+      <c r="C31" t="n">
+        <v>118480</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>58</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BENG03</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>13143</v>
+      </c>
+      <c r="C32" t="n">
+        <v>365066</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>86</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BENG04</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>22658</v>
+      </c>
+      <c r="C33" t="n">
+        <v>803704</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>110</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BENG05</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>35032</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1526570</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>138</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BENG06</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>5832</v>
+      </c>
+      <c r="C35" t="n">
+        <v>108880</v>
+      </c>
+      <c r="D35" t="n">
+        <v>8.596959687012713</v>
+      </c>
+      <c r="E35" t="n">
+        <v>36</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>COMPLETE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BENG07</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>20578</v>
+      </c>
+      <c r="C36" t="n">
+        <v>637304</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>69</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>BENG08</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>44919</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1967996</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>108</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BENG09</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>76913</v>
+      </c>
+      <c r="C38" t="n">
+        <v>4170492</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>130</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>BENG10</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>119757</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8041208</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>168</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>HT10(c4p1)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>9954</v>
+      </c>
+      <c r="C40" t="n">
+        <v>258426</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>64</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>HT11(c4p2)</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>9938</v>
+      </c>
+      <c r="C41" t="n">
+        <v>257498</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>61</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>HT12(c4p3)</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>9955</v>
+      </c>
+      <c r="C42" t="n">
+        <v>258393</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>61</v>
+      </c>
+      <c r="F42" t="inlineStr">
         <is>
           <t>TIMEOUT</t>
         </is>

</xml_diff>

<commit_message>
Implement 2D Strip Packing Problem Solver using Max-SAT approach with rotation support; includes signal handling, checkpointing, and result visualization.
</commit_message>
<xml_diff>
--- a/SPP.xlsx
+++ b/SPP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,20 +468,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HT01(c1p1)</t>
+          <t>CGCUT01</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1015</v>
+        <v>948</v>
       </c>
       <c r="C2" t="n">
-        <v>8680</v>
+        <v>7578</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2652231190004386</v>
+        <v>0.1948401649715379</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -492,68 +492,72 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HT02(c1p2)</t>
+          <t>CGCUT02</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1117</v>
+        <v>3512</v>
       </c>
       <c r="C3" t="n">
-        <v>9853</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.3125638689962216</v>
+        <v>57753</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HT03(c1p3)</t>
+          <t>CGCUT03</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1022</v>
+        <v>50855</v>
       </c>
       <c r="C4" t="n">
-        <v>8792</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.2129374389769509</v>
+        <v>2685933</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E4" t="n">
-        <v>20</v>
+        <v>720</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HT04(c2p1)</t>
+          <t>GCUT01</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2401</v>
+        <v>948</v>
       </c>
       <c r="C5" t="n">
-        <v>30245</v>
+        <v>7578</v>
       </c>
       <c r="D5" t="n">
-        <v>3.673541600001045</v>
+        <v>0.1897847049986012</v>
       </c>
       <c r="E5" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -564,115 +568,119 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HT05(c2p2)</t>
+          <t>GCUT02</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2418</v>
+        <v>3512</v>
       </c>
       <c r="C6" t="n">
-        <v>30680</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4.888466086005792</v>
+        <v>57753</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E6" t="n">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HT06(c2p3)</t>
+          <t>GCUT03</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2416</v>
+        <v>50855</v>
       </c>
       <c r="C7" t="n">
-        <v>30594</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.8519042059779167</v>
+        <v>2685933</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E7" t="n">
-        <v>15</v>
+        <v>720</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HT07(c3p1)</t>
+          <t>GCUT04</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3677</v>
+        <v>157970</v>
       </c>
       <c r="C8" t="n">
-        <v>60998</v>
-      </c>
-      <c r="D8" t="n">
-        <v>14.9961232499918</v>
+        <v>7654725</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E8" t="n">
-        <v>30</v>
+        <v>3170</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HT08(c3p2)</t>
+          <t>NGCUT01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3890</v>
+        <v>439</v>
       </c>
       <c r="C9" t="n">
-        <v>66024</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
+        <v>2635</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2641488290391862</v>
       </c>
       <c r="E9" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>HT09(c3p3)</t>
+          <t>NGCUT02</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3681</v>
+        <v>1128</v>
       </c>
       <c r="C10" t="n">
-        <v>61084</v>
+        <v>9976</v>
       </c>
       <c r="D10" t="n">
-        <v>51.47719361400232</v>
+        <v>1.581005947024096</v>
       </c>
       <c r="E10" t="n">
         <v>30</v>
@@ -686,20 +694,20 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CGCUT01</t>
+          <t>NGCUT03</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>900</v>
+        <v>1548</v>
       </c>
       <c r="C11" t="n">
-        <v>6810</v>
+        <v>14952</v>
       </c>
       <c r="D11" t="n">
-        <v>515.0848403020063</v>
+        <v>0.5304605389828794</v>
       </c>
       <c r="E11" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -710,72 +718,68 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CGCUT02</t>
+          <t>NGCUT04</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3926</v>
+        <v>229</v>
       </c>
       <c r="C12" t="n">
-        <v>67275</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
+        <v>1030</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01609563897363842</v>
       </c>
       <c r="E12" t="n">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CGCUT03</t>
+          <t>NGCUT05</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>90225</v>
+        <v>877</v>
       </c>
       <c r="C13" t="n">
-        <v>5126873</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
+        <v>7207</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.1156697309925221</v>
       </c>
       <c r="E13" t="n">
-        <v>1571</v>
+        <v>36</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GCUT01</t>
+          <t>NGCUT06</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7484</v>
+        <v>941</v>
       </c>
       <c r="C14" t="n">
-        <v>73085</v>
+        <v>7904</v>
       </c>
       <c r="D14" t="n">
-        <v>6.061176014016382</v>
+        <v>10.51251318102004</v>
       </c>
       <c r="E14" t="n">
-        <v>731</v>
+        <v>31</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -786,98 +790,92 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GCUT02</t>
+          <t>NGCUT07</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>26943</v>
+        <v>364</v>
       </c>
       <c r="C15" t="n">
-        <v>523850</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
+        <v>2012</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.03598298702854663</v>
       </c>
       <c r="E15" t="n">
-        <v>1330</v>
+        <v>20</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GCUT03</t>
+          <t>NGCUT08</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>53654</v>
+        <v>832</v>
       </c>
       <c r="C16" t="n">
-        <v>1557855</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
+        <v>6820</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.799220489978325</v>
       </c>
       <c r="E16" t="n">
-        <v>1793</v>
+        <v>33</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GCUT04</t>
+          <t>NGCUT09</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>162970</v>
+        <v>1635</v>
       </c>
       <c r="C17" t="n">
-        <v>7904725</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
+        <v>18469</v>
+      </c>
+      <c r="D17" t="n">
+        <v>519.1112159119803</v>
       </c>
       <c r="E17" t="n">
-        <v>3369</v>
+        <v>51</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>TIMEOUT</t>
+          <t>COMPLETE</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NGCUT01</t>
+          <t>NGCUT10</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>409</v>
+        <v>1353</v>
       </c>
       <c r="C18" t="n">
-        <v>2335</v>
+        <v>13605</v>
       </c>
       <c r="D18" t="n">
-        <v>0.07082334998995066</v>
+        <v>7.238942906958982</v>
       </c>
       <c r="E18" t="n">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -888,20 +886,20 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>NGCUT02</t>
+          <t>NGCUT11</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1094</v>
+        <v>1348</v>
       </c>
       <c r="C19" t="n">
-        <v>9398</v>
+        <v>14025</v>
       </c>
       <c r="D19" t="n">
-        <v>9.377688505977858</v>
+        <v>4.196522652986459</v>
       </c>
       <c r="E19" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -912,14 +910,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NGCUT03</t>
+          <t>NGCUT12</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1548</v>
+        <v>2981</v>
       </c>
       <c r="C20" t="n">
-        <v>14952</v>
+        <v>45407</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -927,7 +925,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -938,20 +936,20 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NGCUT04</t>
+          <t>BENG01</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>201</v>
+        <v>1685</v>
       </c>
       <c r="C21" t="n">
-        <v>834</v>
+        <v>18552</v>
       </c>
       <c r="D21" t="n">
-        <v>0.007145330018829554</v>
+        <v>0.8839333599898964</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -962,116 +960,124 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NGCUT05</t>
+          <t>BENG02</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>863</v>
+        <v>6072</v>
       </c>
       <c r="C22" t="n">
-        <v>7011</v>
-      </c>
-      <c r="D22" t="n">
-        <v>192.9788152209949</v>
+        <v>118480</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E22" t="n">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>NGCUT06</t>
+          <t>BENG03</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>851</v>
+        <v>13143</v>
       </c>
       <c r="C23" t="n">
-        <v>6554</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.2694387389929034</v>
+        <v>365066</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E23" t="n">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NGCUT07</t>
+          <t>BENG04</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>316</v>
+        <v>22658</v>
       </c>
       <c r="C24" t="n">
-        <v>1628</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.02448407997144386</v>
+        <v>803704</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E24" t="n">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>NGCUT08</t>
+          <t>BENG05</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>858</v>
+        <v>35032</v>
       </c>
       <c r="C25" t="n">
-        <v>7158</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1.638874642958399</v>
+        <v>1526570</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E25" t="n">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>NGCUT09</t>
+          <t>BENG06</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1689</v>
+        <v>5832</v>
       </c>
       <c r="C26" t="n">
-        <v>19441</v>
+        <v>108880</v>
       </c>
       <c r="D26" t="n">
-        <v>21.55591251503211</v>
+        <v>7.9147766380338</v>
       </c>
       <c r="E26" t="n">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1082,62 +1088,66 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>NGCUT10</t>
+          <t>BENG07</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1106</v>
+        <v>20578</v>
       </c>
       <c r="C27" t="n">
-        <v>10394</v>
-      </c>
-      <c r="D27" t="n">
-        <v>4.948505807959009</v>
+        <v>637304</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E27" t="n">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NGCUT11</t>
+          <t>BENG08</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1453</v>
+        <v>44919</v>
       </c>
       <c r="C28" t="n">
-        <v>15600</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1.05446800601203</v>
+        <v>1967996</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E28" t="n">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>COMPLETE</t>
+          <t>TIMEOUT</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>NGCUT12</t>
+          <t>BENG09</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2827</v>
+        <v>76593</v>
       </c>
       <c r="C29" t="n">
-        <v>42019</v>
+        <v>4119292</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1145,7 +1155,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1156,332 +1166,24 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BENG01</t>
+          <t>BENG10</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1685</v>
+        <v>118557</v>
       </c>
       <c r="C30" t="n">
-        <v>18552</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.6063239469658583</v>
+        <v>7801208</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>TIMEOUT</t>
+        </is>
       </c>
       <c r="E30" t="n">
-        <v>30</v>
+        <v>169</v>
       </c>
       <c r="F30" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>BENG02</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>6072</v>
-      </c>
-      <c r="C31" t="n">
-        <v>118480</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>58</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>BENG03</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>13143</v>
-      </c>
-      <c r="C32" t="n">
-        <v>365066</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>86</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>BENG04</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>22658</v>
-      </c>
-      <c r="C33" t="n">
-        <v>803704</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>110</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>BENG05</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>35032</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1526570</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
-        <v>138</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>BENG06</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>5832</v>
-      </c>
-      <c r="C35" t="n">
-        <v>108880</v>
-      </c>
-      <c r="D35" t="n">
-        <v>8.596959687012713</v>
-      </c>
-      <c r="E35" t="n">
-        <v>36</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>BENG07</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>20578</v>
-      </c>
-      <c r="C36" t="n">
-        <v>637304</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>69</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>BENG08</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>44919</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1967996</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>108</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>BENG09</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>76913</v>
-      </c>
-      <c r="C38" t="n">
-        <v>4170492</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>130</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>BENG10</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>119757</v>
-      </c>
-      <c r="C39" t="n">
-        <v>8041208</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>168</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>HT10(c4p1)</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>9954</v>
-      </c>
-      <c r="C40" t="n">
-        <v>258426</v>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
-        <v>64</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>HT11(c4p2)</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>9938</v>
-      </c>
-      <c r="C41" t="n">
-        <v>257498</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>61</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>HT12(c4p3)</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>9955</v>
-      </c>
-      <c r="C42" t="n">
-        <v>258393</v>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>TIMEOUT</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>61</v>
-      </c>
-      <c r="F42" t="inlineStr">
         <is>
           <t>TIMEOUT</t>
         </is>

</xml_diff>